<commit_message>
args, dates, projects, persons
</commit_message>
<xml_diff>
--- a/Source/ScanData.xlsx
+++ b/Source/ScanData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sea1693\PycharmProjects\costsheet\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A3B994-E7DE-4976-B6B0-FC4EB9EB914E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178A4C4A-D117-42CC-9DDB-DE24D5217CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{35EC44FF-57E4-4F7B-99B2-D0EF4D2AED57}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{35EC44FF-57E4-4F7B-99B2-D0EF4D2AED57}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
+    <sheet name="Persons" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Официальное наименование проекта</t>
   </si>
@@ -61,6 +62,33 @@
   </si>
   <si>
     <t>Примечание</t>
+  </si>
+  <si>
+    <t>Фамилия</t>
+  </si>
+  <si>
+    <t>ТрЗ без трекинга</t>
+  </si>
+  <si>
+    <t>ID в Yandex Tracker</t>
+  </si>
+  <si>
+    <t>Адолфи</t>
+  </si>
+  <si>
+    <t>raymond</t>
+  </si>
+  <si>
+    <t>Белов</t>
+  </si>
+  <si>
+    <t>belov</t>
+  </si>
+  <si>
+    <t>Буба</t>
+  </si>
+  <si>
+    <t>buba-konskiy</t>
   </si>
 </sst>
 </file>
@@ -425,7 +453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9F27F0-3755-441F-9D45-5A7A37781EA9}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -482,4 +510,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7DD67D-5105-4B2D-AFB0-D9EFACA3E109}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.6328125" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
RELEASE 1.0, drive cache removed
</commit_message>
<xml_diff>
--- a/Source/ScanData.xlsx
+++ b/Source/ScanData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sea1693\PycharmProjects\costsheet\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0079DD-B022-4428-8CC1-763185CF5C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A1548C-3608-4085-B0FB-9D640363EA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{35EC44FF-57E4-4F7B-99B2-D0EF4D2AED57}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Официальное наименование проекта</t>
   </si>
@@ -61,15 +61,6 @@
     <t>Project: "МТ IP1810"</t>
   </si>
   <si>
-    <t>Примечание</t>
-  </si>
-  <si>
-    <t>Фамилия</t>
-  </si>
-  <si>
-    <t>ТрЗ без трекинга</t>
-  </si>
-  <si>
     <t>ID в Yandex Tracker</t>
   </si>
   <si>
@@ -95,6 +86,12 @@
   </si>
   <si>
     <t>potor</t>
+  </si>
+  <si>
+    <t>ТрЗ за смену статуса</t>
+  </si>
+  <si>
+    <t>ФИО</t>
   </si>
 </sst>
 </file>
@@ -460,7 +457,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -476,9 +473,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -487,9 +482,6 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -498,9 +490,6 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -508,9 +497,6 @@
       </c>
       <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -523,33 +509,33 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.6328125" customWidth="1"/>
     <col min="2" max="2" width="21.1796875" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -557,18 +543,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>55</v>
@@ -576,10 +562,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>